<commit_message>
Created Chef Rose card.
</commit_message>
<xml_diff>
--- a/The Rose Card Distribution.xlsx
+++ b/The Rose Card Distribution.xlsx
@@ -365,43 +365,58 @@
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -420,6 +435,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -430,24 +448,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -836,7 +836,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,183 +849,183 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="20"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="14" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="G5" s="14" t="s">
+      <c r="E5" s="20"/>
+      <c r="G5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="15"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="5">
         <v>1</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="8">
         <v>4</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="8">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="A8" s="4">
         <v>0</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="5">
         <v>1</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="8">
         <v>2</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="8">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+      <c r="A9" s="4">
         <v>1</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="5">
         <v>11</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="8">
         <v>5</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="8">
         <v>2</v>
       </c>
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="11">
-        <v>1</v>
-      </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+      <c r="A11" s="4">
         <v>3</v>
       </c>
-      <c r="B11" s="8">
-        <v>1</v>
-      </c>
-      <c r="D11" s="29" t="s">
+      <c r="B11" s="5">
+        <v>2</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="D12" s="13" t="s">
+      <c r="B12" s="5"/>
+      <c r="D12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="10"/>
+      <c r="B13" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Updated card distribution + New chart to display all individual card info.
</commit_message>
<xml_diff>
--- a/The Rose Card Distribution.xlsx
+++ b/The Rose Card Distribution.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="70">
   <si>
     <t>The Rose Card Distribution</t>
   </si>
@@ -78,6 +78,162 @@
   </si>
   <si>
     <t>Special</t>
+  </si>
+  <si>
+    <t>Card Name</t>
+  </si>
+  <si>
+    <t>Card Cost</t>
+  </si>
+  <si>
+    <t>Card Text</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Beak Dive</t>
+  </si>
+  <si>
+    <t>Can only be played when in flight. Deal 25 (35) damage. Lose all flight.</t>
+  </si>
+  <si>
+    <t>Beak Drill</t>
+  </si>
+  <si>
+    <t>Deal (X times 2) times 1 (2) damage.</t>
+  </si>
+  <si>
+    <t>Belly Bump</t>
+  </si>
+  <si>
+    <t>Deal damage equal to the number of Food items eaten this combat. Quarter(Halve) the counter.</t>
+  </si>
+  <si>
+    <t>Chef Rose</t>
+  </si>
+  <si>
+    <t>Deal !D! Damage. Add a random (Upgraded) Food item to your hand.</t>
+  </si>
+  <si>
+    <t>Defend</t>
+  </si>
+  <si>
+    <t>Gain 5 (8) Block.</t>
+  </si>
+  <si>
+    <t>Donut</t>
+  </si>
+  <si>
+    <t>Draw 1 Card. Lose 1 Flight. Exhaust.</t>
+  </si>
+  <si>
+    <t>Gain 1 energy. Gain 1 Flight. Exhaust.</t>
+  </si>
+  <si>
+    <t>Energy Drink</t>
+  </si>
+  <si>
+    <t>Flipper Flap</t>
+  </si>
+  <si>
+    <t>Deal 1 damage 2 (3) times. Exhaust.</t>
+  </si>
+  <si>
+    <t>Deck Archetype</t>
+  </si>
+  <si>
+    <t>Flight</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Fly High to the Sky!</t>
+  </si>
+  <si>
+    <t>Gain 1 Penguin Flight.</t>
+  </si>
+  <si>
+    <t>Fried Chicken</t>
+  </si>
+  <si>
+    <t>Gain 2 Strength. At the end of this turn, lose 2 Strength. Exhaust.</t>
+  </si>
+  <si>
+    <t>Hamburger</t>
+  </si>
+  <si>
+    <t>Gain 6 Block. This card counts as 3 Food items. Exhaust.</t>
+  </si>
+  <si>
+    <t>Hungry Form</t>
+  </si>
+  <si>
+    <t>At the start of your turn, consume 1 (2) random food item(s).</t>
+  </si>
+  <si>
+    <t>Peck</t>
+  </si>
+  <si>
+    <t>Apply 1 vulnerable. If in flight, apply 1 (2) weak too.</t>
+  </si>
+  <si>
+    <t>Reorder</t>
+  </si>
+  <si>
+    <t>Return all Exhausted Food items to your hand. Exhaust.</t>
+  </si>
+  <si>
+    <t>Sharing Is Caring</t>
+  </si>
+  <si>
+    <t>Food/Passivity</t>
+  </si>
+  <si>
+    <t>Apply 3 Bribe for the number of Food items in your hand. Exhaust all Food items.</t>
+  </si>
+  <si>
+    <t>Strike</t>
+  </si>
+  <si>
+    <t>Deal 6 (9) damage.</t>
+  </si>
+  <si>
+    <t>Sushi</t>
+  </si>
+  <si>
+    <t>Heal 1. Exhaust.</t>
+  </si>
+  <si>
+    <t>Takesies Backsies</t>
+  </si>
+  <si>
+    <t>For every !M! Bribe, reduce Bribe by !M!, deal !D! damage, and consume a random Food item.</t>
+  </si>
+  <si>
+    <t>Temper Tantrum</t>
+  </si>
+  <si>
+    <t>At the start of every turn, add a Flipper Flap to your hand.</t>
+  </si>
+  <si>
+    <t>UberDishes</t>
+  </si>
+  <si>
+    <t>Create 2 random (upgraded) food items in your discard pile.</t>
+  </si>
+  <si>
+    <t>Work Out</t>
+  </si>
+  <si>
+    <t>Gain 1 (2) Strength.</t>
   </si>
 </sst>
 </file>
@@ -179,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -351,6 +507,80 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -363,7 +593,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -449,6 +679,43 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -552,19 +819,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table24" displayName="Table24" ref="D6:E12" totalsRowCount="1" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="D6:E11"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Rarity" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="3"/>
-    <tableColumn id="2" name="The Rose" totalsRowLabel="0" dataDxfId="8" totalsRowDxfId="2"/>
+    <tableColumn id="1" name="Rarity" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="2" name="The Rose" totalsRowLabel="0" dataDxfId="7" totalsRowDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table244" displayName="Table244" ref="G6:H10" totalsRowCount="1" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table244" displayName="Table244" ref="G6:H10" totalsRowCount="1" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="G6:H9"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Rarity" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="1"/>
-    <tableColumn id="2" name="The Rose" totalsRowLabel="0" dataDxfId="4" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Rarity" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="The Rose" totalsRowLabel="0" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -833,22 +1100,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26:J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="5" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="5" customWidth="1"/>
     <col min="7" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="47.5703125" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -860,7 +1131,7 @@
       <c r="G1" s="22"/>
       <c r="H1" s="23"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -870,7 +1141,7 @@
       <c r="G2" s="25"/>
       <c r="H2" s="26"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27"/>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
@@ -880,7 +1151,7 @@
       <c r="G3" s="28"/>
       <c r="H3" s="29"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>1</v>
       </c>
@@ -895,7 +1166,7 @@
       </c>
       <c r="H5" s="20"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -915,7 +1186,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -935,7 +1206,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>0</v>
       </c>
@@ -955,7 +1226,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -975,7 +1246,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>2</v>
       </c>
@@ -995,7 +1266,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>3</v>
       </c>
@@ -1009,7 +1280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -1021,14 +1292,668 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="7"/>
     </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="43"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="32">
+        <v>3</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="38"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="36"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="34">
+        <v>1</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="36"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="34">
+        <v>1</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="36"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="34">
+        <v>1</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="36"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="34">
+        <v>1</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="36"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="34">
+        <v>1</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="36"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="34">
+        <v>0</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="36"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="34">
+        <v>2</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="36"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="34">
+        <v>1</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="36"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="34">
+        <v>1</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="36"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="34">
+        <v>3</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="36"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="34">
+        <v>1</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="36"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="34">
+        <v>3</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="36"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="34">
+        <v>1</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="36"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="34">
+        <v>1</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="36"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="44">
+        <v>1</v>
+      </c>
+      <c r="C32" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="34">
+        <v>2</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="G34" s="48"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="34">
+        <v>1</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="34">
+        <v>1</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G36" s="48"/>
+      <c r="H36" s="48"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="48"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="48"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="34"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="48"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="48"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="34"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="48"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="48"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="34"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="48"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="48"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="48"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="48"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="34">
+    <mergeCell ref="F31:J31"/>
+    <mergeCell ref="F32:J32"/>
+    <mergeCell ref="F33:J33"/>
+    <mergeCell ref="F34:J34"/>
+    <mergeCell ref="F35:J35"/>
+    <mergeCell ref="F36:J36"/>
+    <mergeCell ref="F37:J37"/>
+    <mergeCell ref="F38:J38"/>
+    <mergeCell ref="F39:J39"/>
+    <mergeCell ref="F40:J40"/>
+    <mergeCell ref="F41:J41"/>
+    <mergeCell ref="F42:J42"/>
+    <mergeCell ref="F43:J43"/>
+    <mergeCell ref="F44:J44"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="F21:J21"/>
+    <mergeCell ref="F22:J22"/>
+    <mergeCell ref="F23:J23"/>
+    <mergeCell ref="F24:J24"/>
+    <mergeCell ref="F25:J25"/>
+    <mergeCell ref="F26:J26"/>
+    <mergeCell ref="F27:J27"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="F29:J29"/>
+    <mergeCell ref="F30:J30"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="G5:H5"/>

</xml_diff>

<commit_message>
Fixed small table error.
</commit_message>
<xml_diff>
--- a/The Rose Card Distribution.xlsx
+++ b/The Rose Card Distribution.xlsx
@@ -593,7 +593,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -695,28 +695,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
@@ -1102,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:J26"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,13 +1313,13 @@
       <c r="E15" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="41" t="s">
+      <c r="F15" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="43"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="49"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
@@ -1338,13 +1337,13 @@
       <c r="E16" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="38"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="36"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
@@ -1359,16 +1358,16 @@
       <c r="D17" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="44" t="s">
+      <c r="E17" s="40" t="s">
         <v>40</v>
       </c>
       <c r="F17" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="36"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="38"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
@@ -1383,16 +1382,16 @@
       <c r="D18" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="44" t="s">
+      <c r="E18" s="40" t="s">
         <v>41</v>
       </c>
       <c r="F18" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="36"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
@@ -1407,16 +1406,16 @@
       <c r="D19" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="45" t="s">
+      <c r="E19" s="41" t="s">
         <v>41</v>
       </c>
       <c r="F19" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="36"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="38"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
@@ -1431,16 +1430,16 @@
       <c r="D20" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="45" t="s">
+      <c r="E20" s="41" t="s">
         <v>42</v>
       </c>
       <c r="F20" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="36"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
@@ -1455,16 +1454,16 @@
       <c r="D21" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="45" t="s">
+      <c r="E21" s="41" t="s">
         <v>41</v>
       </c>
       <c r="F21" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="36"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="38"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
@@ -1479,16 +1478,16 @@
       <c r="D22" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="45" t="s">
+      <c r="E22" s="41" t="s">
         <v>41</v>
       </c>
       <c r="F22" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="36"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="38"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
@@ -1503,16 +1502,16 @@
       <c r="D23" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="45" t="s">
+      <c r="E23" s="41" t="s">
         <v>40</v>
       </c>
       <c r="F23" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="36"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="38"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
@@ -1533,10 +1532,10 @@
       <c r="F24" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="36"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
@@ -1557,10 +1556,10 @@
       <c r="F25" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="36"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="38"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
@@ -1581,10 +1580,10 @@
       <c r="F26" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="36"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="38"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
@@ -1605,10 +1604,10 @@
       <c r="F27" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="36"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
@@ -1629,10 +1628,10 @@
       <c r="F28" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="36"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
@@ -1653,10 +1652,10 @@
       <c r="F29" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="36"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
@@ -1677,10 +1676,10 @@
       <c r="F30" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="36"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
@@ -1701,34 +1700,34 @@
       <c r="F31" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="36"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="44">
+      <c r="B32" s="40">
         <v>1</v>
       </c>
-      <c r="C32" s="44" t="s">
+      <c r="C32" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="44" t="s">
+      <c r="D32" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="44" t="s">
+      <c r="E32" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="F32" s="47" t="s">
+      <c r="F32" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="44"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="34" t="s">
@@ -1746,13 +1745,13 @@
       <c r="E33" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="F33" s="48" t="s">
+      <c r="F33" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="48"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="38"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="34" t="s">
@@ -1770,13 +1769,13 @@
       <c r="E34" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F34" s="48" t="s">
+      <c r="F34" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="38"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="34" t="s">
@@ -1794,13 +1793,13 @@
       <c r="E35" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="F35" s="48" t="s">
+      <c r="F35" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
-      <c r="J35" s="48"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="38"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="34" t="s">
@@ -1818,13 +1817,13 @@
       <c r="E36" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="48" t="s">
+      <c r="F36" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="G36" s="48"/>
-      <c r="H36" s="48"/>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="38"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="34"/>
@@ -1832,11 +1831,11 @@
       <c r="C37" s="34"/>
       <c r="D37" s="34"/>
       <c r="E37" s="34"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="48"/>
-      <c r="H37" s="48"/>
-      <c r="I37" s="48"/>
-      <c r="J37" s="48"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="38"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="34"/>
@@ -1844,11 +1843,11 @@
       <c r="C38" s="34"/>
       <c r="D38" s="34"/>
       <c r="E38" s="34"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
-      <c r="I38" s="48"/>
-      <c r="J38" s="48"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="38"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="34"/>
@@ -1856,11 +1855,11 @@
       <c r="C39" s="34"/>
       <c r="D39" s="34"/>
       <c r="E39" s="34"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="38"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="34"/>
@@ -1868,11 +1867,11 @@
       <c r="C40" s="34"/>
       <c r="D40" s="34"/>
       <c r="E40" s="34"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48"/>
-      <c r="I40" s="48"/>
-      <c r="J40" s="48"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="38"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="34"/>
@@ -1880,11 +1879,11 @@
       <c r="C41" s="34"/>
       <c r="D41" s="34"/>
       <c r="E41" s="34"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="48"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="38"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="34"/>
@@ -1892,11 +1891,11 @@
       <c r="C42" s="34"/>
       <c r="D42" s="34"/>
       <c r="E42" s="34"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="38"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="34"/>
@@ -1904,11 +1903,11 @@
       <c r="C43" s="34"/>
       <c r="D43" s="34"/>
       <c r="E43" s="34"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="38"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="34"/>
@@ -1916,44 +1915,17 @@
       <c r="C44" s="34"/>
       <c r="D44" s="34"/>
       <c r="E44" s="34"/>
-      <c r="F44" s="48"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="F31:J31"/>
-    <mergeCell ref="F32:J32"/>
-    <mergeCell ref="F33:J33"/>
-    <mergeCell ref="F34:J34"/>
-    <mergeCell ref="F35:J35"/>
-    <mergeCell ref="F36:J36"/>
-    <mergeCell ref="F37:J37"/>
-    <mergeCell ref="F38:J38"/>
-    <mergeCell ref="F39:J39"/>
-    <mergeCell ref="F40:J40"/>
-    <mergeCell ref="F41:J41"/>
-    <mergeCell ref="F42:J42"/>
-    <mergeCell ref="F43:J43"/>
-    <mergeCell ref="F44:J44"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="F21:J21"/>
-    <mergeCell ref="F22:J22"/>
-    <mergeCell ref="F23:J23"/>
-    <mergeCell ref="F24:J24"/>
-    <mergeCell ref="F25:J25"/>
-    <mergeCell ref="F26:J26"/>
-    <mergeCell ref="F27:J27"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="F29:J29"/>
-    <mergeCell ref="F30:J30"/>
+  <sortState ref="A16:F36">
+    <sortCondition ref="A16"/>
+  </sortState>
+  <mergeCells count="4">
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="G5:H5"/>

</xml_diff>

<commit_message>
Created Head Pat card.
</commit_message>
<xml_diff>
--- a/The Rose Card Distribution.xlsx
+++ b/The Rose Card Distribution.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="73">
   <si>
     <t>The Rose Card Distribution</t>
   </si>
@@ -234,6 +234,15 @@
   </si>
   <si>
     <t>Gain 1 (2) Strength.</t>
+  </si>
+  <si>
+    <t>Head Pat</t>
+  </si>
+  <si>
+    <t>Deal !D! damage. Apply !M! Passivity.</t>
+  </si>
+  <si>
+    <t>Passivity</t>
   </si>
 </sst>
 </file>
@@ -641,45 +650,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -716,6 +686,45 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
@@ -1101,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G39" sqref="G38:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,51 +1128,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="46"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="49"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="18"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="G5" s="19" t="s">
+      <c r="E5" s="40"/>
+      <c r="G5" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="20"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -1298,628 +1307,640 @@
       <c r="B13" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="47" t="s">
+      <c r="F15" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="49"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="36"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="19">
         <v>3</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="43" t="s">
+      <c r="F16" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="36"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="23"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="39" t="s">
+      <c r="F17" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="38"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="25"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="34">
+      <c r="B18" s="21">
         <v>1</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="39" t="s">
+      <c r="F18" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="38"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="25"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="34">
+      <c r="B19" s="21">
         <v>1</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="41" t="s">
+      <c r="E19" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="39" t="s">
+      <c r="F19" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="38"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="25"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="34">
+      <c r="B20" s="21">
         <v>1</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="39" t="s">
+      <c r="F20" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="38"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="25"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="34">
+      <c r="B21" s="21">
         <v>1</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="39" t="s">
+      <c r="F21" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="38"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="25"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="34">
+      <c r="B22" s="21">
         <v>1</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="41" t="s">
+      <c r="E22" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="38"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="25"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="34">
+      <c r="B23" s="21">
         <v>0</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="41" t="s">
+      <c r="E23" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="38"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="25"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="34">
+      <c r="B24" s="21">
         <v>2</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="39" t="s">
+      <c r="F24" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="38"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="25"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="34">
+      <c r="B25" s="21">
         <v>1</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="E25" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="39" t="s">
+      <c r="F25" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="38"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="25"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="34">
+      <c r="B26" s="21">
         <v>1</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="34" t="s">
+      <c r="E26" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="F26" s="39" t="s">
+      <c r="F26" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="38"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="25"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="34">
+      <c r="B27" s="21">
         <v>3</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="39" t="s">
+      <c r="F27" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="38"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="25"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="34">
+      <c r="B28" s="21">
         <v>1</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="34" t="s">
+      <c r="E28" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="39" t="s">
+      <c r="F28" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="38"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="34">
+      <c r="B29" s="21">
         <v>3</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="D29" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="34" t="s">
+      <c r="E29" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="F29" s="39" t="s">
+      <c r="F29" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="38"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="34">
+      <c r="B30" s="21">
         <v>1</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="34" t="s">
+      <c r="D30" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="34" t="s">
+      <c r="E30" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="39" t="s">
+      <c r="F30" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="38"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="25"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="34">
+      <c r="B31" s="21">
         <v>1</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="D31" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="39" t="s">
+      <c r="F31" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="38"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="25"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="42" t="s">
+      <c r="A32" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="40">
+      <c r="B32" s="27">
         <v>1</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="40" t="s">
+      <c r="E32" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="F32" s="45" t="s">
+      <c r="F32" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="44"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="31"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="34">
+      <c r="B33" s="21">
         <v>2</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="34" t="s">
+      <c r="E33" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F33" s="39" t="s">
+      <c r="F33" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="38"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="25"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="34">
+      <c r="B34" s="21">
         <v>1</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D34" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="E34" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="F34" s="39" t="s">
+      <c r="F34" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="38"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="25"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="34">
+      <c r="B35" s="21">
         <v>1</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="34" t="s">
+      <c r="D35" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E35" s="34" t="s">
+      <c r="E35" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="F35" s="39" t="s">
+      <c r="F35" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="38"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="25"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="34">
+      <c r="B36" s="21">
         <v>1</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="34" t="s">
+      <c r="D36" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="34" t="s">
+      <c r="E36" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="39" t="s">
+      <c r="F36" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="38"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="25"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="34"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="38"/>
+      <c r="A37" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="21">
+        <v>0</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="25"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="34"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="38"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="25"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="34"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="38"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="25"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="38"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="25"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="34"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="38"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="25"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="34"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="38"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="37"/>
-      <c r="J43" s="38"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="25"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="37"/>
-      <c r="J44" s="38"/>
+      <c r="A44" s="21"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="25"/>
     </row>
   </sheetData>
   <sortState ref="A16:F36">

</xml_diff>

<commit_message>
Small card detail fixes.
</commit_message>
<xml_diff>
--- a/The Rose Card Distribution.xlsx
+++ b/The Rose Card Distribution.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="75">
   <si>
     <t>The Rose Card Distribution</t>
   </si>
@@ -243,6 +243,12 @@
   </si>
   <si>
     <t>Passivity</t>
+  </si>
+  <si>
+    <t>Stay Still</t>
+  </si>
+  <si>
+    <t>Can only be played if no Attack was played. Apply !M! Passivity. End your turn.</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1117,7 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G39" sqref="G38:G39"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,12 +1865,24 @@
       <c r="J37" s="25"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="26"/>
+      <c r="A38" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="21">
+        <v>1</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>74</v>
+      </c>
       <c r="G38" s="24"/>
       <c r="H38" s="24"/>
       <c r="I38" s="24"/>

</xml_diff>

<commit_message>
Changed Beak Dive to Uncommon, base damage down by 10.
</commit_message>
<xml_diff>
--- a/The Rose Card Distribution.xlsx
+++ b/The Rose Card Distribution.xlsx
@@ -95,9 +95,6 @@
     <t>Beak Dive</t>
   </si>
   <si>
-    <t>Can only be played when in flight. Deal 25 (35) damage. Lose all flight.</t>
-  </si>
-  <si>
     <t>Beak Drill</t>
   </si>
   <si>
@@ -255,6 +252,9 @@
   </si>
   <si>
     <t>Can only be played if no Food item was played this turn and not in Flight. Draw !M! Cards.</t>
+  </si>
+  <si>
+    <t>Can only be played when in flight. Deal 15 (20) damage. Lose all flight.</t>
   </si>
 </sst>
 </file>
@@ -1122,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,7 +1332,7 @@
         <v>21</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>20</v>
@@ -1347,19 +1347,19 @@
         <v>22</v>
       </c>
       <c r="B16" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>4</v>
@@ -1380,10 +1380,10 @@
         <v>14</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="21">
         <v>1</v>
@@ -1404,10 +1404,10 @@
         <v>14</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G18" s="24"/>
       <c r="H18" s="24"/>
@@ -1416,7 +1416,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="21">
         <v>1</v>
@@ -1428,10 +1428,10 @@
         <v>14</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
@@ -1440,7 +1440,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="21">
         <v>1</v>
@@ -1452,10 +1452,10 @@
         <v>15</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="21">
         <v>1</v>
@@ -1476,10 +1476,10 @@
         <v>15</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G21" s="24"/>
       <c r="H21" s="24"/>
@@ -1488,7 +1488,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="21">
         <v>1</v>
@@ -1500,10 +1500,10 @@
         <v>15</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G22" s="24"/>
       <c r="H22" s="24"/>
@@ -1512,7 +1512,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="21">
         <v>0</v>
@@ -1524,10 +1524,10 @@
         <v>14</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="21">
         <v>2</v>
@@ -1548,10 +1548,10 @@
         <v>15</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F24" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="21">
         <v>1</v>
@@ -1572,10 +1572,10 @@
         <v>15</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F25" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G25" s="24"/>
       <c r="H25" s="24"/>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="21">
         <v>1</v>
@@ -1596,10 +1596,10 @@
         <v>15</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G26" s="24"/>
       <c r="H26" s="24"/>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" s="21">
         <v>3</v>
@@ -1620,10 +1620,10 @@
         <v>16</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F27" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="21">
         <v>1</v>
@@ -1644,10 +1644,10 @@
         <v>14</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F28" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G28" s="24"/>
       <c r="H28" s="24"/>
@@ -1656,7 +1656,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29" s="21">
         <v>3</v>
@@ -1668,10 +1668,10 @@
         <v>15</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F29" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G29" s="24"/>
       <c r="H29" s="24"/>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="21">
         <v>1</v>
@@ -1692,10 +1692,10 @@
         <v>15</v>
       </c>
       <c r="E30" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="26" t="s">
         <v>56</v>
-      </c>
-      <c r="F30" s="26" t="s">
-        <v>57</v>
       </c>
       <c r="G30" s="24"/>
       <c r="H30" s="24"/>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" s="21">
         <v>1</v>
@@ -1716,10 +1716,10 @@
         <v>14</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F31" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G31" s="24"/>
       <c r="H31" s="24"/>
@@ -1728,7 +1728,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" s="27">
         <v>1</v>
@@ -1740,10 +1740,10 @@
         <v>15</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G32" s="33"/>
       <c r="H32" s="33"/>
@@ -1752,7 +1752,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33" s="21">
         <v>2</v>
@@ -1764,10 +1764,10 @@
         <v>14</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G33" s="24"/>
       <c r="H33" s="24"/>
@@ -1776,7 +1776,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="21">
         <v>1</v>
@@ -1788,10 +1788,10 @@
         <v>16</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F34" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G34" s="24"/>
       <c r="H34" s="24"/>
@@ -1800,7 +1800,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" s="21">
         <v>1</v>
@@ -1812,10 +1812,10 @@
         <v>15</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F35" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G35" s="24"/>
       <c r="H35" s="24"/>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" s="21">
         <v>1</v>
@@ -1836,10 +1836,10 @@
         <v>16</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F36" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G36" s="24"/>
       <c r="H36" s="24"/>
@@ -1848,7 +1848,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B37" s="21">
         <v>0</v>
@@ -1860,10 +1860,10 @@
         <v>14</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F37" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G37" s="24"/>
       <c r="H37" s="24"/>
@@ -1872,7 +1872,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B38" s="21">
         <v>1</v>
@@ -1884,10 +1884,10 @@
         <v>15</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G38" s="24"/>
       <c r="H38" s="24"/>
@@ -1896,7 +1896,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39" s="21">
         <v>1</v>
@@ -1908,10 +1908,10 @@
         <v>15</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F39" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G39" s="24"/>
       <c r="H39" s="24"/>

</xml_diff>

<commit_message>
Updated to reflect recently tweaked/rebalanced cards Fly, Peck.
</commit_message>
<xml_diff>
--- a/The Rose Card Distribution.xlsx
+++ b/The Rose Card Distribution.xlsx
@@ -1123,7 +1123,7 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1638,7 +1638,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D28" s="21" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Reworked Flipper Flap to deal damage to random enemies.
</commit_message>
<xml_diff>
--- a/The Rose Card Distribution.xlsx
+++ b/The Rose Card Distribution.xlsx
@@ -134,9 +134,6 @@
     <t>Flipper Flap</t>
   </si>
   <si>
-    <t>Deal 1 damage 2 (3) times. Exhaust.</t>
-  </si>
-  <si>
     <t>Deck Archetype</t>
   </si>
   <si>
@@ -255,6 +252,9 @@
   </si>
   <si>
     <t>Can only be played when in flight. Deal 15 (20) damage. Lose all flight.</t>
+  </si>
+  <si>
+    <t>Deal 1 damage to a random enemy 2 (3) times. Exhaust.</t>
   </si>
 </sst>
 </file>
@@ -1122,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,7 +1332,7 @@
         <v>21</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>20</v>
@@ -1356,10 +1356,10 @@
         <v>14</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
@@ -1380,7 +1380,7 @@
         <v>14</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" s="26" t="s">
         <v>24</v>
@@ -1404,7 +1404,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="26" t="s">
         <v>26</v>
@@ -1428,7 +1428,7 @@
         <v>14</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="26" t="s">
         <v>28</v>
@@ -1452,7 +1452,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F20" s="26" t="s">
         <v>30</v>
@@ -1476,7 +1476,7 @@
         <v>15</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F21" s="26" t="s">
         <v>32</v>
@@ -1500,7 +1500,7 @@
         <v>15</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F22" s="26" t="s">
         <v>33</v>
@@ -1524,10 +1524,10 @@
         <v>14</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
@@ -1536,22 +1536,22 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D24" s="21" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F24" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="21">
         <v>1</v>
@@ -1572,10 +1572,10 @@
         <v>15</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F25" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G25" s="24"/>
       <c r="H25" s="24"/>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="21">
         <v>1</v>
@@ -1596,10 +1596,10 @@
         <v>15</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G26" s="24"/>
       <c r="H26" s="24"/>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" s="21">
         <v>3</v>
@@ -1620,10 +1620,10 @@
         <v>16</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" s="21">
         <v>1</v>
@@ -1644,10 +1644,10 @@
         <v>14</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F28" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G28" s="24"/>
       <c r="H28" s="24"/>
@@ -1656,7 +1656,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="21">
         <v>3</v>
@@ -1668,10 +1668,10 @@
         <v>15</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F29" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G29" s="24"/>
       <c r="H29" s="24"/>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30" s="21">
         <v>1</v>
@@ -1692,10 +1692,10 @@
         <v>15</v>
       </c>
       <c r="E30" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F30" s="26" t="s">
         <v>55</v>
-      </c>
-      <c r="F30" s="26" t="s">
-        <v>56</v>
       </c>
       <c r="G30" s="24"/>
       <c r="H30" s="24"/>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" s="21">
         <v>1</v>
@@ -1716,10 +1716,10 @@
         <v>14</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F31" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G31" s="24"/>
       <c r="H31" s="24"/>
@@ -1728,7 +1728,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="27">
         <v>1</v>
@@ -1740,10 +1740,10 @@
         <v>15</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G32" s="33"/>
       <c r="H32" s="33"/>
@@ -1752,7 +1752,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="21">
         <v>2</v>
@@ -1764,10 +1764,10 @@
         <v>14</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F33" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G33" s="24"/>
       <c r="H33" s="24"/>
@@ -1776,7 +1776,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="21">
         <v>1</v>
@@ -1788,10 +1788,10 @@
         <v>16</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F34" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G34" s="24"/>
       <c r="H34" s="24"/>
@@ -1800,7 +1800,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" s="21">
         <v>1</v>
@@ -1812,10 +1812,10 @@
         <v>15</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F35" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G35" s="24"/>
       <c r="H35" s="24"/>
@@ -1824,7 +1824,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B36" s="21">
         <v>1</v>
@@ -1836,10 +1836,10 @@
         <v>16</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F36" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G36" s="24"/>
       <c r="H36" s="24"/>
@@ -1848,7 +1848,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B37" s="21">
         <v>0</v>
@@ -1860,10 +1860,10 @@
         <v>14</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F37" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G37" s="24"/>
       <c r="H37" s="24"/>
@@ -1872,7 +1872,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B38" s="21">
         <v>1</v>
@@ -1884,10 +1884,10 @@
         <v>15</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G38" s="24"/>
       <c r="H38" s="24"/>
@@ -1896,7 +1896,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B39" s="21">
         <v>1</v>
@@ -1908,10 +1908,10 @@
         <v>15</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F39" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G39" s="24"/>
       <c r="H39" s="24"/>

</xml_diff>

<commit_message>
Changed Stay Still to apply to all enemies.
</commit_message>
<xml_diff>
--- a/The Rose Card Distribution.xlsx
+++ b/The Rose Card Distribution.xlsx
@@ -242,9 +242,6 @@
     <t>Stay Still</t>
   </si>
   <si>
-    <t>Can only be played if no Attack was played. Apply !M! Passivity. End your turn.</t>
-  </si>
-  <si>
     <t>Sprint</t>
   </si>
   <si>
@@ -255,6 +252,9 @@
   </si>
   <si>
     <t>Deal 1 damage to a random enemy 2 (3) times. Exhaust.</t>
+  </si>
+  <si>
+    <t>Can only be played if no Attack was played. Apply !M! Passivity to all enemies. End your turn.</t>
   </si>
 </sst>
 </file>
@@ -1122,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,7 +1359,7 @@
         <v>37</v>
       </c>
       <c r="F16" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
@@ -1527,7 +1527,7 @@
         <v>38</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
@@ -1887,7 +1887,7 @@
         <v>70</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G38" s="24"/>
       <c r="H38" s="24"/>
@@ -1896,7 +1896,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B39" s="21">
         <v>1</v>
@@ -1911,7 +1911,7 @@
         <v>40</v>
       </c>
       <c r="F39" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G39" s="24"/>
       <c r="H39" s="24"/>

</xml_diff>

<commit_message>
Changed Peck type to Skill.
</commit_message>
<xml_diff>
--- a/The Rose Card Distribution.xlsx
+++ b/The Rose Card Distribution.xlsx
@@ -1122,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1641,7 +1641,7 @@
         <v>9</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E28" s="21" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Created A Fish A Day card.
</commit_message>
<xml_diff>
--- a/The Rose Card Distribution.xlsx
+++ b/The Rose Card Distribution.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="86">
   <si>
     <t>The Rose Card Distribution</t>
   </si>
@@ -260,6 +260,18 @@
   </si>
   <si>
     <t>Gain !M! Flight. Add a random Food item to your hand.</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>If an enemy does not intend to attack, apply !M! Passivity. Increase this card's Passivity by !theRose:SecondMagic! for this combat.</t>
+  </si>
+  <si>
+    <t>A Fish A Day!</t>
+  </si>
+  <si>
+    <t>Gain !M! Artifact. At the end of this turn, lose !M! Artifact. Exhaust.</t>
   </si>
 </sst>
 </file>
@@ -1684,8 +1696,8 @@
   <sheetPr/>
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1698,6 +1710,7 @@
     <col min="6" max="6" width="5" customWidth="1"/>
     <col min="7" max="8" width="12.8518518518519" customWidth="1"/>
     <col min="9" max="9" width="47.5740740740741" customWidth="1"/>
+    <col min="10" max="10" width="28.6666666666667" customWidth="1"/>
     <col min="13" max="13" width="9.13888888888889" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2529,24 +2542,48 @@
       <c r="J41" s="48"/>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="38"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="40"/>
+      <c r="A42" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="38">
+        <v>1</v>
+      </c>
+      <c r="C42" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="F42" s="40" t="s">
+        <v>83</v>
+      </c>
       <c r="G42" s="41"/>
       <c r="H42" s="41"/>
       <c r="I42" s="41"/>
       <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="38"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="40"/>
+      <c r="A43" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="38">
+        <v>1</v>
+      </c>
+      <c r="C43" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="F43" s="40" t="s">
+        <v>85</v>
+      </c>
       <c r="G43" s="41"/>
       <c r="H43" s="41"/>
       <c r="I43" s="41"/>

</xml_diff>

<commit_message>
Updated to reflect latest balance changes.
</commit_message>
<xml_diff>
--- a/The Rose Card Distribution.xlsx
+++ b/The Rose Card Distribution.xlsx
@@ -196,7 +196,7 @@
     <t>Fried Chicken</t>
   </si>
   <si>
-    <t>Gain 2 Strength. At the end of this turn, lose 2 Strength. Exhaust.</t>
+    <t>Gain 1 Strength. At the end of this turn, lose 1 Strength. Exhaust.</t>
   </si>
   <si>
     <t>Hamburger</t>
@@ -226,7 +226,7 @@
     <t>Sushi</t>
   </si>
   <si>
-    <t>Gain 2 Dexterity. At the end of this turn, lose 2 Dexterity. Exhaust.</t>
+    <t>Gain 1 Dexterity. At the end of this turn, lose 1 Dexterity. Exhaust.</t>
   </si>
   <si>
     <t>UberDishes</t>
@@ -1696,8 +1696,8 @@
   <sheetPr/>
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Updated to reflect Fly High to The Sky! buffs.
</commit_message>
<xml_diff>
--- a/The Rose Card Distribution.xlsx
+++ b/The Rose Card Distribution.xlsx
@@ -190,7 +190,7 @@
     <t>Fly High to the Sky!</t>
   </si>
   <si>
-    <t>Gain 1 Penguin Flight.</t>
+    <t>Gain 3 Block. Gain 1 Penguin Flight.</t>
   </si>
   <si>
     <t>Fried Chicken</t>
@@ -279,9 +279,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* \-??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
@@ -315,9 +315,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -332,18 +360,18 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -355,46 +383,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -414,15 +407,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -436,10 +428,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -457,14 +465,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -517,163 +517,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -932,6 +932,89 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -950,93 +1033,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1054,124 +1054,124 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="36" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1697,7 +1697,7 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>